<commit_message>
new excel sheet added
</commit_message>
<xml_diff>
--- a/assets/certificate.xlsx
+++ b/assets/certificate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8592"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="244">
   <si>
     <t>S.NO</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Devika BR</t>
   </si>
   <si>
-    <t>9400301761</t>
-  </si>
-  <si>
     <t>devikaraveendran0@gmail.com</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>Gowri mohan</t>
   </si>
   <si>
-    <t>8943862081</t>
-  </si>
-  <si>
     <t>gowrimohan8620@gmail.com</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>Gouri M Biju</t>
   </si>
   <si>
-    <t>7736702081</t>
-  </si>
-  <si>
     <t>gourigourimbiju@gmail.com</t>
   </si>
   <si>
@@ -379,9 +370,6 @@
     <t>Archana S</t>
   </si>
   <si>
-    <t>9400930260</t>
-  </si>
-  <si>
     <t>archanasanel10@gmail.com</t>
   </si>
   <si>
@@ -481,9 +469,6 @@
     <t>Aswathy Ashok</t>
   </si>
   <si>
-    <t>8129574840</t>
-  </si>
-  <si>
     <t>aswathyashok912@gmail.com</t>
   </si>
   <si>
@@ -499,9 +484,6 @@
     <t>Nesla</t>
   </si>
   <si>
-    <t>8590929802</t>
-  </si>
-  <si>
     <t>nesla2332004@gmail.com</t>
   </si>
   <si>
@@ -526,9 +508,6 @@
     <t>Abhiram m p</t>
   </si>
   <si>
-    <t>7510274318</t>
-  </si>
-  <si>
     <t>abhiram4318@gmail.com</t>
   </si>
   <si>
@@ -580,9 +559,6 @@
     <t>Abhiram Renjith</t>
   </si>
   <si>
-    <t>8089311685</t>
-  </si>
-  <si>
     <t>abhiramrenjith967@gmail.com</t>
   </si>
   <si>
@@ -706,9 +682,6 @@
     <t>Arun Krishna K U</t>
   </si>
   <si>
-    <t>9633082570</t>
-  </si>
-  <si>
     <t>arunkrishnaku2019@gmail.com</t>
   </si>
   <si>
@@ -740,9 +713,6 @@
   </si>
   <si>
     <t>Ebrahim Roshan U</t>
-  </si>
-  <si>
-    <t>9961840533</t>
   </si>
   <si>
     <t>roshandzire021@gmail.com</t>
@@ -786,10 +756,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -814,6 +784,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -828,45 +813,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -881,10 +829,26 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -900,14 +864,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -929,7 +885,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -937,7 +900,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -966,7 +936,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,19 +1002,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,25 +1074,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,121 +1116,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1157,6 +1127,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1171,32 +1156,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1234,6 +1193,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1260,148 +1230,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1791,13 +1761,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.71296296296296" customWidth="1"/>
     <col min="2" max="2" width="14.287037037037" customWidth="1"/>
@@ -2156,7 +2126,7 @@
         <v>53489325</v>
       </c>
     </row>
-    <row r="14" ht="14.4" spans="1:8">
+    <row r="14" ht="14.4" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2172,15 +2142,18 @@
       <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>940030761</v>
+      </c>
+      <c r="G14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
       <c r="H14">
         <f t="shared" si="0"/>
         <v>53489326</v>
+      </c>
+      <c r="I14">
+        <v>9400301761</v>
       </c>
     </row>
     <row r="15" ht="14.4" spans="1:8">
@@ -2191,7 +2164,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -2200,17 +2173,17 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
         <v>51</v>
       </c>
-      <c r="G15" t="s">
-        <v>52</v>
-      </c>
       <c r="H15">
         <f t="shared" si="0"/>
         <v>53489327</v>
       </c>
     </row>
-    <row r="16" ht="14.4" spans="1:8">
+    <row r="16" ht="14.4" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2218,7 +2191,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -2226,15 +2199,18 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F16" t="s">
-        <v>54</v>
+      <c r="F16">
+        <v>894362081</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
         <v>53489328</v>
+      </c>
+      <c r="I16">
+        <v>8943862081</v>
       </c>
     </row>
     <row r="17" ht="14.4" spans="1:8">
@@ -2245,7 +2221,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -2254,10 +2230,10 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
@@ -2272,7 +2248,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2281,10 +2257,10 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
@@ -2299,7 +2275,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -2308,10 +2284,10 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
@@ -2326,19 +2302,19 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="G20" t="s">
         <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" t="s">
-        <v>68</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
@@ -2353,7 +2329,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -2362,10 +2338,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
@@ -2380,10 +2356,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -2392,7 +2368,7 @@
         <v>8606976517</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
@@ -2407,7 +2383,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -2416,10 +2392,10 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
@@ -2434,7 +2410,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -2443,10 +2419,10 @@
         <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
@@ -2461,19 +2437,19 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
         <v>80</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" t="s">
-        <v>82</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
@@ -2488,7 +2464,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>33</v>
@@ -2497,17 +2473,17 @@
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
         <v>53489338</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:8">
+    <row r="27" ht="15.75" customHeight="1" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2515,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
@@ -2523,15 +2499,18 @@
       <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" t="s">
-        <v>87</v>
+      <c r="F27">
+        <v>776702081</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
         <v>53489339</v>
+      </c>
+      <c r="I27">
+        <v>7736702081</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" spans="1:8">
@@ -2542,7 +2521,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
@@ -2551,10 +2530,10 @@
         <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
@@ -2569,7 +2548,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
         <v>33</v>
@@ -2578,10 +2557,10 @@
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
@@ -2596,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -2605,10 +2584,10 @@
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
@@ -2623,7 +2602,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>33</v>
@@ -2635,7 +2614,7 @@
         <v>9847568852</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
@@ -2650,7 +2629,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -2659,10 +2638,10 @@
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
@@ -2677,7 +2656,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
         <v>33</v>
@@ -2686,10 +2665,10 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
@@ -2704,7 +2683,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
         <v>33</v>
@@ -2713,10 +2692,10 @@
         <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
@@ -2731,19 +2710,19 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" t="s">
         <v>109</v>
-      </c>
-      <c r="D35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>111</v>
-      </c>
-      <c r="G35" t="s">
-        <v>112</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
@@ -2758,19 +2737,19 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
@@ -2785,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
@@ -2794,17 +2773,17 @@
         <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
         <v>53489349</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1" spans="1:8">
+    <row r="38" ht="15.75" customHeight="1" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2812,7 +2791,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
         <v>33</v>
@@ -2820,15 +2799,18 @@
       <c r="E38" t="s">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
-        <v>120</v>
+      <c r="F38">
+        <v>940930260</v>
       </c>
       <c r="G38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
         <v>53489350</v>
+      </c>
+      <c r="I38">
+        <v>9400930260</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1" spans="1:8">
@@ -2839,7 +2821,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
         <v>33</v>
@@ -2848,10 +2830,10 @@
         <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
@@ -2866,10 +2848,10 @@
         <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
         <v>11</v>
@@ -2878,7 +2860,7 @@
         <v>9946730277</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
@@ -2893,19 +2875,19 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
         <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
@@ -2920,7 +2902,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D42" t="s">
         <v>33</v>
@@ -2929,10 +2911,10 @@
         <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H42">
         <f t="shared" si="0"/>
@@ -2947,7 +2929,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
@@ -2956,10 +2938,10 @@
         <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
@@ -2974,7 +2956,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s">
         <v>33</v>
@@ -2983,10 +2965,10 @@
         <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
@@ -3001,7 +2983,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
         <v>33</v>
@@ -3010,10 +2992,10 @@
         <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
@@ -3028,7 +3010,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
         <v>33</v>
@@ -3037,10 +3019,10 @@
         <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G46" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
@@ -3055,19 +3037,19 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E47" t="s">
         <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H47">
         <f t="shared" si="0"/>
@@ -3082,7 +3064,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
@@ -3094,7 +3076,7 @@
         <v>9539244272</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
@@ -3109,26 +3091,26 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E49" t="s">
         <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H49">
         <f t="shared" si="0"/>
         <v>53489361</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1" spans="1:8">
+    <row r="50" ht="15.75" customHeight="1" spans="1:9">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3136,7 +3118,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D50" t="s">
         <v>33</v>
@@ -3144,15 +3126,18 @@
       <c r="E50" t="s">
         <v>11</v>
       </c>
-      <c r="F50" t="s">
-        <v>154</v>
+      <c r="F50">
+        <v>812957440</v>
       </c>
       <c r="G50" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H50">
         <f t="shared" si="0"/>
         <v>53489362</v>
+      </c>
+      <c r="I50">
+        <v>8129574840</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1" spans="1:8">
@@ -3163,26 +3148,26 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
         <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G51" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H51">
         <f t="shared" si="0"/>
         <v>53489363</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1" spans="1:8">
+    <row r="52" ht="15.75" customHeight="1" spans="1:9">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3190,23 +3175,26 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
       </c>
-      <c r="F52" t="s">
-        <v>160</v>
+      <c r="F52">
+        <v>859092902</v>
       </c>
       <c r="G52" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H52">
         <f t="shared" si="0"/>
         <v>53489364</v>
+      </c>
+      <c r="I52">
+        <v>8590929802</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" spans="1:8">
@@ -3217,19 +3205,19 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H53">
         <f t="shared" si="0"/>
@@ -3244,7 +3232,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
@@ -3253,17 +3241,17 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G54" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H54">
         <f t="shared" si="0"/>
         <v>53489366</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1" spans="1:8">
+    <row r="55" ht="15.75" customHeight="1" spans="1:9">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3271,7 +3259,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>33</v>
@@ -3279,15 +3267,18 @@
       <c r="E55" t="s">
         <v>11</v>
       </c>
-      <c r="F55" t="s">
-        <v>169</v>
+      <c r="F55">
+        <v>751027418</v>
       </c>
       <c r="G55" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H55">
         <f t="shared" si="0"/>
         <v>53489367</v>
+      </c>
+      <c r="I55">
+        <v>7510274318</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1" spans="1:8">
@@ -3298,7 +3289,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D56" t="s">
         <v>33</v>
@@ -3307,10 +3298,10 @@
         <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G56" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H56">
         <f t="shared" si="0"/>
@@ -3325,7 +3316,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
         <v>33</v>
@@ -3334,10 +3325,10 @@
         <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G57" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H57">
         <f t="shared" si="0"/>
@@ -3352,7 +3343,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -3361,10 +3352,10 @@
         <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G58" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H58">
         <f t="shared" si="0"/>
@@ -3379,19 +3370,19 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
         <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G59" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H59">
         <f t="shared" si="0"/>
@@ -3406,19 +3397,19 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E60" t="s">
         <v>11</v>
       </c>
       <c r="F60" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G60" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H60">
         <f t="shared" si="0"/>
@@ -3433,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
         <v>33</v>
@@ -3441,11 +3432,11 @@
       <c r="E61" t="s">
         <v>11</v>
       </c>
-      <c r="F61" t="s">
-        <v>187</v>
+      <c r="F61">
+        <v>8089311685</v>
       </c>
       <c r="G61" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H61">
         <f t="shared" si="0"/>
@@ -3460,19 +3451,19 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E62" t="s">
         <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="G62" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H62">
         <f t="shared" si="0"/>
@@ -3487,19 +3478,19 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E63" t="s">
         <v>11</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="G63" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H63">
         <f t="shared" si="0"/>
@@ -3514,7 +3505,7 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D64" t="s">
         <v>33</v>
@@ -3523,10 +3514,10 @@
         <v>11</v>
       </c>
       <c r="F64" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G64" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
@@ -3541,7 +3532,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D65" t="s">
         <v>33</v>
@@ -3550,10 +3541,10 @@
         <v>11</v>
       </c>
       <c r="F65" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G65" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H65">
         <f t="shared" si="0"/>
@@ -3568,19 +3559,19 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E66" t="s">
         <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G66" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H66">
         <f t="shared" si="0"/>
@@ -3595,22 +3586,22 @@
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
         <v>11</v>
       </c>
       <c r="F67" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="G67" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H67">
-        <f>H66+1</f>
+        <f t="shared" ref="H67:H72" si="1">H66+1</f>
         <v>53489379</v>
       </c>
     </row>
@@ -3622,22 +3613,22 @@
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D68" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E68" t="s">
         <v>11</v>
       </c>
       <c r="F68" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G68" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H68">
-        <f>H67+1</f>
+        <f t="shared" si="1"/>
         <v>53489380</v>
       </c>
     </row>
@@ -3649,7 +3640,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D69" t="s">
         <v>33</v>
@@ -3658,13 +3649,13 @@
         <v>11</v>
       </c>
       <c r="F69" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G69" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H69">
-        <f>H68+1</f>
+        <f t="shared" si="1"/>
         <v>53489381</v>
       </c>
     </row>
@@ -3676,7 +3667,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s">
         <v>33</v>
@@ -3685,13 +3676,13 @@
         <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G70" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H70">
-        <f>H69+1</f>
+        <f t="shared" si="1"/>
         <v>53489382</v>
       </c>
     </row>
@@ -3703,22 +3694,22 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E71" t="s">
         <v>11</v>
       </c>
       <c r="F71" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="G71" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H71">
-        <f>H70+1</f>
+        <f t="shared" si="1"/>
         <v>53489383</v>
       </c>
     </row>
@@ -3730,22 +3721,22 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E72" t="s">
         <v>11</v>
       </c>
       <c r="F72" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G72" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H72">
-        <f>H71+1</f>
+        <f t="shared" si="1"/>
         <v>53489384</v>
       </c>
     </row>
@@ -3757,19 +3748,19 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D73" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E73" t="s">
         <v>11</v>
       </c>
       <c r="F73" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G73" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H73" t="e">
         <f>#REF!+1</f>
@@ -3784,7 +3775,7 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -3793,17 +3784,17 @@
         <v>11</v>
       </c>
       <c r="F74" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="G74" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H74" t="e">
         <f>H73+1</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1" spans="1:8">
+    <row r="75" ht="15.75" customHeight="1" spans="1:9">
       <c r="A75">
         <v>75</v>
       </c>
@@ -3811,24 +3802,27 @@
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D75" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E75" t="s">
         <v>11</v>
       </c>
-      <c r="F75" t="s">
-        <v>229</v>
+      <c r="F75">
+        <v>963082570</v>
       </c>
       <c r="G75" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H75" t="e">
         <f>H74+1</f>
         <v>#REF!</v>
       </c>
+      <c r="I75">
+        <v>9633082570</v>
+      </c>
     </row>
     <row r="76" ht="15.75" customHeight="1" spans="1:8">
       <c r="A76">
@@ -3838,7 +3832,7 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D76" t="s">
         <v>33</v>
@@ -3847,10 +3841,10 @@
         <v>11</v>
       </c>
       <c r="F76" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="G76" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="H76" t="e">
         <f>H75+1</f>
@@ -3865,19 +3859,19 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E77" t="s">
         <v>11</v>
       </c>
       <c r="F77" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G77" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="H77" t="e">
         <f>H76+1</f>
@@ -3892,26 +3886,26 @@
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E78" t="s">
         <v>11</v>
       </c>
       <c r="F78" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G78" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H78" t="e">
         <f>H77+1</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="79" ht="15.75" customHeight="1" spans="1:8">
+    <row r="79" ht="15.75" customHeight="1" spans="1:9">
       <c r="A79">
         <v>81</v>
       </c>
@@ -3919,7 +3913,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s">
         <v>33</v>
@@ -3927,16 +3921,19 @@
       <c r="E79" t="s">
         <v>11</v>
       </c>
-      <c r="F79" t="s">
-        <v>241</v>
+      <c r="F79">
+        <v>996184053</v>
       </c>
       <c r="G79" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="H79" t="e">
         <f>#REF!+1</f>
         <v>#REF!</v>
       </c>
+      <c r="I79">
+        <v>9961840533</v>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1" spans="1:8">
       <c r="A80">
@@ -3946,7 +3943,7 @@
         <v>8</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>33</v>
@@ -3958,7 +3955,7 @@
         <v>7510941531</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="H80" t="e">
         <f>H79+1</f>
@@ -3973,19 +3970,19 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D81" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E81" t="s">
         <v>11</v>
       </c>
       <c r="F81" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="G81" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="H81" t="e">
         <f>#REF!+1</f>
@@ -4000,7 +3997,7 @@
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D82" t="s">
         <v>33</v>
@@ -4009,10 +4006,10 @@
         <v>11</v>
       </c>
       <c r="F82" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="G82" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="H82" t="e">
         <f>H81+1</f>
@@ -4027,7 +4024,7 @@
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D83" t="s">
         <v>33</v>
@@ -4036,10 +4033,10 @@
         <v>11</v>
       </c>
       <c r="F83" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G83" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="H83" t="e">
         <f>H82+1</f>

</xml_diff>